<commit_message>
Proof reading and making edits
</commit_message>
<xml_diff>
--- a/index/figure/Abbreviations/Abbreviations.xlsx
+++ b/index/figure/Abbreviations/Abbreviations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lg14289_bristol_ac_uk/Documents/PhD/Main project/Thesis/index/figure/Abbreviations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC3A83B2-8E43-3B43-9E70-93FBA90CCB81}"/>
+  <xr:revisionPtr revIDLastSave="328" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07770A84-4B87-0D4A-BDC2-3F05EF358C38}"/>
   <bookViews>
-    <workbookView xWindow="15520" yWindow="460" windowWidth="10000" windowHeight="14840" xr2:uid="{5A89F498-7711-DB48-901A-56700D0ABE21}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="20480" windowHeight="12300" xr2:uid="{5A89F498-7711-DB48-901A-56700D0ABE21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="284">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -280,6 +280,612 @@
   </si>
   <si>
     <t>Alcohol dehydrogenase</t>
+  </si>
+  <si>
+    <t>RCT</t>
+  </si>
+  <si>
+    <t>Randomised control trial</t>
+  </si>
+  <si>
+    <t>CHD</t>
+  </si>
+  <si>
+    <t>Coronary heart disease</t>
+  </si>
+  <si>
+    <t>DXA</t>
+  </si>
+  <si>
+    <t>Dual-energy X-ray Absorptiometry</t>
+  </si>
+  <si>
+    <t>VTE</t>
+  </si>
+  <si>
+    <t>Venous thromboembolism</t>
+  </si>
+  <si>
+    <t>DVT</t>
+  </si>
+  <si>
+    <t>Deep vein thrombosis</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Pulmonary embolism</t>
+  </si>
+  <si>
+    <t>IHD</t>
+  </si>
+  <si>
+    <t>Ischaemic heart disease</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>Coronary artery disease</t>
+  </si>
+  <si>
+    <t>WHRadjBMI</t>
+  </si>
+  <si>
+    <t>Waist-hip ratio adjusted for BMI</t>
+  </si>
+  <si>
+    <t>MACE</t>
+  </si>
+  <si>
+    <t>Major adverse cardiovascular event</t>
+  </si>
+  <si>
+    <t>T2D</t>
+  </si>
+  <si>
+    <t>Type 2 Diabetes mellitus</t>
+  </si>
+  <si>
+    <t>PGI2</t>
+  </si>
+  <si>
+    <t>Prostaglandin I2</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Nitric oxide</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Glycoprotein</t>
+  </si>
+  <si>
+    <t>PAR-1</t>
+  </si>
+  <si>
+    <t>Protease-activated receptor 1</t>
+  </si>
+  <si>
+    <t>PAR1-activating peptide</t>
+  </si>
+  <si>
+    <t>PAR1-AP/TRAP-6</t>
+  </si>
+  <si>
+    <t>IP3</t>
+  </si>
+  <si>
+    <t>Inositol trisphosphate</t>
+  </si>
+  <si>
+    <t>PKC</t>
+  </si>
+  <si>
+    <t>Protein kinase C</t>
+  </si>
+  <si>
+    <t>PCI</t>
+  </si>
+  <si>
+    <t>Percutaneous coronary intervention</t>
+  </si>
+  <si>
+    <t>DAPT</t>
+  </si>
+  <si>
+    <t>Dual antiplatelet therapy</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>Adenosine diphosphate</t>
+  </si>
+  <si>
+    <t>LTA</t>
+  </si>
+  <si>
+    <t>Light transmittance aggregometry</t>
+  </si>
+  <si>
+    <t>PLC</t>
+  </si>
+  <si>
+    <t>Phospholipase C</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Phosphatidylserine</t>
+  </si>
+  <si>
+    <t>PSGL-1</t>
+  </si>
+  <si>
+    <t>P-selectin glycoprotein ligand-1</t>
+  </si>
+  <si>
+    <t>GPCR</t>
+  </si>
+  <si>
+    <t>G protein coupled receptor</t>
+  </si>
+  <si>
+    <t>PKA</t>
+  </si>
+  <si>
+    <t>Protien kinase A</t>
+  </si>
+  <si>
+    <t>PGE1</t>
+  </si>
+  <si>
+    <t>Prostaglandin E1</t>
+  </si>
+  <si>
+    <t>VASP</t>
+  </si>
+  <si>
+    <t>Vasodilator-stimulator phosphoprotein</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Mass spectrometry</t>
+  </si>
+  <si>
+    <t>IGF-1</t>
+  </si>
+  <si>
+    <t>Insulin-like growth factor 1</t>
+  </si>
+  <si>
+    <t>PKB</t>
+  </si>
+  <si>
+    <t>Protein kinase B</t>
+  </si>
+  <si>
+    <t>TxA2</t>
+  </si>
+  <si>
+    <t>Thromboxane A2</t>
+  </si>
+  <si>
+    <t>PI3K</t>
+  </si>
+  <si>
+    <t>Phosphoinositde-3-kinase</t>
+  </si>
+  <si>
+    <t>TPO</t>
+  </si>
+  <si>
+    <t>Thrombopoietin</t>
+  </si>
+  <si>
+    <t>MAPK</t>
+  </si>
+  <si>
+    <t>Mitogen-activated protein kinase</t>
+  </si>
+  <si>
+    <t>CCR4</t>
+  </si>
+  <si>
+    <t>C-C motif chemokine receptor 4</t>
+  </si>
+  <si>
+    <t>ERK</t>
+  </si>
+  <si>
+    <t>Extracellular signal regulated kinase</t>
+  </si>
+  <si>
+    <t>WAT</t>
+  </si>
+  <si>
+    <t>White adipose tissue</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>Brown adipose tissue</t>
+  </si>
+  <si>
+    <t>IL-6</t>
+  </si>
+  <si>
+    <t>Interleukin-6</t>
+  </si>
+  <si>
+    <t>TNF-⍺</t>
+  </si>
+  <si>
+    <t>Tumour necrosis factor-⍺</t>
+  </si>
+  <si>
+    <t>pQTL</t>
+  </si>
+  <si>
+    <t>Protein quantitative trait loci</t>
+  </si>
+  <si>
+    <t>IL6R</t>
+  </si>
+  <si>
+    <t>Interleukin-6 receptor</t>
+  </si>
+  <si>
+    <t>ELISA</t>
+  </si>
+  <si>
+    <t>Enzyme-linked immunosorbent assay</t>
+  </si>
+  <si>
+    <t>National Health Service Blood and Transplant</t>
+  </si>
+  <si>
+    <t>GIANT</t>
+  </si>
+  <si>
+    <t>Genetic Investigation of Anthromopetric Traits</t>
+  </si>
+  <si>
+    <t>EDTA</t>
+  </si>
+  <si>
+    <t>Ethylenediamine tetraacetic acid</t>
+  </si>
+  <si>
+    <t>GAM</t>
+  </si>
+  <si>
+    <t>Generalized additive model</t>
+  </si>
+  <si>
+    <t>MEA</t>
+  </si>
+  <si>
+    <t>Multiple electrode aggregometry</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Area under the curve</t>
+  </si>
+  <si>
+    <t>Metabolic syndrome</t>
+  </si>
+  <si>
+    <t>TMT-MS</t>
+  </si>
+  <si>
+    <t>Tandem mass tag mass spectrometry</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>Bicinchoninic acid</t>
+  </si>
+  <si>
+    <t>ACD</t>
+  </si>
+  <si>
+    <t>Acid citrate dextrose</t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t>Sodium dodecyl sulphate</t>
+  </si>
+  <si>
+    <t>TBS</t>
+  </si>
+  <si>
+    <t>Tris buffered saline</t>
+  </si>
+  <si>
+    <t>IRAS</t>
+  </si>
+  <si>
+    <t>Integrated Research Application System</t>
+  </si>
+  <si>
+    <t>RIPA</t>
+  </si>
+  <si>
+    <t>Radioimmunoprecipitation assay</t>
+  </si>
+  <si>
+    <t>NSAID</t>
+  </si>
+  <si>
+    <t>Non-steroidal anti-inflammatory drug</t>
+  </si>
+  <si>
+    <t>TEMED</t>
+  </si>
+  <si>
+    <t>Tetramethylethylenediamine</t>
+  </si>
+  <si>
+    <t>BSA</t>
+  </si>
+  <si>
+    <t>Bovine serum albumin</t>
+  </si>
+  <si>
+    <t>PRP</t>
+  </si>
+  <si>
+    <t>Platelet rich plasma</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>Revolutions per minute</t>
+  </si>
+  <si>
+    <t>RFU</t>
+  </si>
+  <si>
+    <t>Relative fluorescent units</t>
+  </si>
+  <si>
+    <t>PFA</t>
+  </si>
+  <si>
+    <t>Paraformaldehyde</t>
+  </si>
+  <si>
+    <t>MFI</t>
+  </si>
+  <si>
+    <t>Median fluorescence intensity</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Arbitrary Units</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>False discovery rate</t>
+  </si>
+  <si>
+    <t>EC50</t>
+  </si>
+  <si>
+    <t>Half maximal effective concentration</t>
+  </si>
+  <si>
+    <t>pEC50</t>
+  </si>
+  <si>
+    <t>The negative logarithm of the EC50</t>
+  </si>
+  <si>
+    <t>ACTB</t>
+  </si>
+  <si>
+    <t>Actin</t>
+  </si>
+  <si>
+    <t>MPO</t>
+  </si>
+  <si>
+    <t>Myeloperoxidase</t>
+  </si>
+  <si>
+    <t>S100A9/MRP-14</t>
+  </si>
+  <si>
+    <t>Myeloid-related protein-14</t>
+  </si>
+  <si>
+    <t>APMAP</t>
+  </si>
+  <si>
+    <t>Adipocyte plasma membrane-associated protein</t>
+  </si>
+  <si>
+    <t>GRK6</t>
+  </si>
+  <si>
+    <t>G protein-coupled receptor kinase 6</t>
+  </si>
+  <si>
+    <t>MMP-2</t>
+  </si>
+  <si>
+    <t>Metalloproteinase-2</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>Platelet poor plasma</t>
+  </si>
+  <si>
+    <t>PBS</t>
+  </si>
+  <si>
+    <t>Phoshate-buffered saline</t>
+  </si>
+  <si>
+    <t>DTT</t>
+  </si>
+  <si>
+    <t>Dithiothreitol</t>
+  </si>
+  <si>
+    <t>PDVF</t>
+  </si>
+  <si>
+    <t>Poly(vinylidene fluoride)</t>
+  </si>
+  <si>
+    <t>IVW</t>
+  </si>
+  <si>
+    <t>Inverse variance weighted</t>
+  </si>
+  <si>
+    <t>ROCK</t>
+  </si>
+  <si>
+    <t>Rho-associated protein kinase</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Quality control</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>Gene ontology</t>
+  </si>
+  <si>
+    <t>PAFAH</t>
+  </si>
+  <si>
+    <t>Platelet-activating factor acetylhydrolase</t>
+  </si>
+  <si>
+    <t>PECAM-1</t>
+  </si>
+  <si>
+    <t>Platelet endothelial cell adhesion molecule-1</t>
+  </si>
+  <si>
+    <t>PDGF</t>
+  </si>
+  <si>
+    <t>Platelet-derived growth factor</t>
+  </si>
+  <si>
+    <t>PEAR1</t>
+  </si>
+  <si>
+    <t>Platelet endothelial aggregation receptor 1</t>
+  </si>
+  <si>
+    <t>GHR</t>
+  </si>
+  <si>
+    <t>Growth hormone receptor</t>
+  </si>
+  <si>
+    <t>SCAR5</t>
+  </si>
+  <si>
+    <t>Scavenger receptor class A member 5</t>
+  </si>
+  <si>
+    <t>PTPRU</t>
+  </si>
+  <si>
+    <t>Receptor-type tyrosine-protein phosphatase U</t>
+  </si>
+  <si>
+    <t>CHAD</t>
+  </si>
+  <si>
+    <t>Chondroadherin</t>
+  </si>
+  <si>
+    <t>CBPM</t>
+  </si>
+  <si>
+    <t>Carboxypeptidase M</t>
+  </si>
+  <si>
+    <t>ADH4</t>
+  </si>
+  <si>
+    <t>Alcohol dehydrogenase 4</t>
+  </si>
+  <si>
+    <t>FHS</t>
+  </si>
+  <si>
+    <t>Framingham Heart Study</t>
+  </si>
+  <si>
+    <t>VLED</t>
+  </si>
+  <si>
+    <t>Very low energy diet</t>
+  </si>
+  <si>
+    <t>INHBC</t>
+  </si>
+  <si>
+    <t>Inhibin β C chain</t>
+  </si>
+  <si>
+    <t>PROTACs</t>
+  </si>
+  <si>
+    <t>Proteolysis targeting chimeras</t>
+  </si>
+  <si>
+    <t>NLMR</t>
+  </si>
+  <si>
+    <t>GLSMR</t>
+  </si>
+  <si>
+    <t>GAM and linear stratified Mendelian randomisation</t>
+  </si>
+  <si>
+    <t>Nonlinear Mendelian randomisation</t>
+  </si>
+  <si>
+    <t>LACE</t>
+  </si>
+  <si>
+    <t>Localised average causal effect</t>
   </si>
 </sst>
 </file>
@@ -650,16 +1256,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363B8D67-7BC3-2B44-A7ED-E4979080C323}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -990,6 +1596,830 @@
         <v>81</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B111" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B114" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>228</v>
+      </c>
+      <c r="B116" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>236</v>
+      </c>
+      <c r="B120" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>250</v>
+      </c>
+      <c r="B128" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>252</v>
+      </c>
+      <c r="B129" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>254</v>
+      </c>
+      <c r="B130" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>256</v>
+      </c>
+      <c r="B131" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>258</v>
+      </c>
+      <c r="B132" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>260</v>
+      </c>
+      <c r="B133" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>262</v>
+      </c>
+      <c r="B134" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>264</v>
+      </c>
+      <c r="B135" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>266</v>
+      </c>
+      <c r="B136" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>268</v>
+      </c>
+      <c r="B137" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>270</v>
+      </c>
+      <c r="B138" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>272</v>
+      </c>
+      <c r="B139" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>274</v>
+      </c>
+      <c r="B140" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>276</v>
+      </c>
+      <c r="B141" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>282</v>
+      </c>
+      <c r="B144" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added acknowledgements in, added chapter 9 to abstract and linked findings back to aims in the discussion chapter
</commit_message>
<xml_diff>
--- a/index/figure/Abbreviations/Abbreviations.xlsx
+++ b/index/figure/Abbreviations/Abbreviations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lg14289_bristol_ac_uk/Documents/PhD/Main project/Thesis/index/figure/Abbreviations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DEA9B5-6C2E-0B4E-8508-FF9337C5AE33}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD6E9FB-699B-6045-A5BE-99515D58441A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="12300" xr2:uid="{5A89F498-7711-DB48-901A-56700D0ABE21}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="287">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -165,9 +165,6 @@
     <t>NHSBT</t>
   </si>
   <si>
-    <t>NHS Blood and Transplant</t>
-  </si>
-  <si>
     <t>Slow Off-rate Modified Aptamers</t>
   </si>
   <si>
@@ -892,6 +889,12 @@
   </si>
   <si>
     <t>Plasminogen activator inhibitor-1</t>
+  </si>
+  <si>
+    <t>CVD</t>
+  </si>
+  <si>
+    <t>Cardiovascular disease</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363B8D67-7BC3-2B44-A7ED-E4979080C323}">
-  <dimension ref="A1:B145"/>
+  <dimension ref="A1:B144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,9 +1447,9 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1455,268 +1458,268 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
         <v>111</v>
@@ -1727,236 +1730,236 @@
         <v>113</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B74" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="B86" t="s">
         <v>171</v>
@@ -1964,47 +1967,47 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>181</v>
+        <v>139</v>
       </c>
       <c r="B92" t="s">
         <v>182</v>
@@ -2012,426 +2015,418 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B97" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B100" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B102" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B104" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B105" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B106" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B107" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B108" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B109" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B110" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B111" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B112" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B113" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B114" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>226</v>
+      <c r="A115" t="s">
+        <v>227</v>
       </c>
       <c r="B115" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B116" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B117" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B118" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B119" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B120" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B121" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B122" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B123" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>65</v>
+        <v>251</v>
       </c>
       <c r="B127" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B128" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B129" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B130" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B131" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B133" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B134" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B135" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B136" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B137" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B138" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B139" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B140" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B141" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B142" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B143" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B144" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>284</v>
-      </c>
-      <c r="B145" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Examiner comments Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/index/figure/Abbreviations/Abbreviations.xlsx
+++ b/index/figure/Abbreviations/Abbreviations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lg14289_bristol_ac_uk/Documents/PhD/Main project/Thesis/index/figure/Abbreviations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CD6E9FB-699B-6045-A5BE-99515D58441A}"/>
+  <xr:revisionPtr revIDLastSave="340" documentId="8_{40A8CF05-02E5-3A43-9EB9-9A1E66D63E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B0821CD-594E-FC4B-B0FF-32311C9A12D9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="12300" xr2:uid="{5A89F498-7711-DB48-901A-56700D0ABE21}"/>
+    <workbookView xWindow="8840" yWindow="-16080" windowWidth="20480" windowHeight="12300" xr2:uid="{5A89F498-7711-DB48-901A-56700D0ABE21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="291">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -895,6 +895,18 @@
   </si>
   <si>
     <t>Cardiovascular disease</t>
+  </si>
+  <si>
+    <t>tPA</t>
+  </si>
+  <si>
+    <t>Tissue plasminogen activator</t>
+  </si>
+  <si>
+    <t>PAF</t>
+  </si>
+  <si>
+    <t>Platelet-activating factor</t>
   </si>
 </sst>
 </file>
@@ -1265,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363B8D67-7BC3-2B44-A7ED-E4979080C323}">
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2429,6 +2441,22 @@
         <v>286</v>
       </c>
     </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>287</v>
+      </c>
+      <c r="B145" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>289</v>
+      </c>
+      <c r="B146" t="s">
+        <v>290</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>